<commit_message>
Mise à jour de la COTS List
</commit_message>
<xml_diff>
--- a/01.byd-DataFactory/1.ArchitectureDossier/artifacts/02.cots-list/BYD-DF_COTSLists_v01.00.xlsx
+++ b/01.byd-DataFactory/1.ArchitectureDossier/artifacts/02.cots-list/BYD-DF_COTSLists_v01.00.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xavierwuelche/Documents/Projet/byd-all-documentation/01.byd-DataFactory/1.ArchitectureDossier/artifacts/02.cots-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179CE4FD-81FE-2242-9B4D-101E6CBB1858}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50505BFC-5635-7F42-85A1-D7CA72E7567A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="33600" windowHeight="19120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="33600" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01 - COTS List" sheetId="5" r:id="rId1"/>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="92">
   <si>
     <t>Description</t>
   </si>
@@ -428,13 +428,28 @@
   </si>
   <si>
     <t>PostGIS is a spatial database extender for PostgreSQL object-relational database. It adds support for geographic objects allowing location queries to be run in SQL.</t>
+  </si>
+  <si>
+    <t>dotenv</t>
+  </si>
+  <si>
+    <t>6.*.*</t>
+  </si>
+  <si>
+    <t>https://www.npmjs.com/package/dotenv</t>
+  </si>
+  <si>
+    <t>BSD-2-Clause</t>
+  </si>
+  <si>
+    <t>Dotenv is a zero-dependency module that loads environment variables from a .env file into process.env</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,8 +608,15 @@
       <color theme="1"/>
       <name val="IBM Plex Sans"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -622,6 +644,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -730,7 +758,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -822,7 +850,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -834,6 +861,16 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="3" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1231,9 +1268,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1251,7 +1288,7 @@
     <row r="1" spans="1:9" s="1" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="14" t="str">
         <f>"COTS List - ("&amp;COUNTA(B5:B85)&amp;" Registered)"</f>
-        <v>COTS List - (21 Registered)</v>
+        <v>COTS List - (22 Registered)</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1392,23 +1429,23 @@
     </row>
     <row r="10" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>12</v>
+      <c r="B10" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>23</v>
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="30"/>
@@ -1416,61 +1453,61 @@
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="24" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="23" t="s">
+      <c r="B12" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="23" t="s">
-        <v>42</v>
+      <c r="F12" s="26" t="s">
+        <v>39</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>44</v>
+        <v>15</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>41</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G13" s="23" t="s">
         <v>23</v>
@@ -1479,80 +1516,80 @@
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="28" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="23" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="28" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>8</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="21"/>
+        <v>48</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-      <c r="B16" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="21" t="s">
+      <c r="B16" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>23</v>
-      </c>
+      <c r="F16" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="21"/>
     </row>
     <row r="17" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="B17" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="23" t="s">
+      <c r="B17" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="23" t="s">
-        <v>54</v>
+      <c r="F17" s="22" t="s">
+        <v>9</v>
       </c>
       <c r="G17" s="23" t="s">
         <v>23</v>
@@ -1561,19 +1598,19 @@
     <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="28" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G18" s="23" t="s">
         <v>23</v>
@@ -1582,156 +1619,168 @@
     <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="28" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>60</v>
+        <v>14</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>56</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
-      <c r="B20" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="E20" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="F20" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="G20" s="34" t="s">
-        <v>78</v>
+      <c r="B20" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
-      <c r="B21" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="F21" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="G21" s="34" t="s">
+      <c r="B21" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="33" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
-      <c r="B22" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>68</v>
+      <c r="B22" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="25" t="s">
+      <c r="B23" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="26" t="s">
-        <v>67</v>
+      <c r="F23" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="21" t="s">
+      <c r="B24" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="G24" s="23"/>
+      <c r="F24" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="G25" s="23"/>
+    </row>
+    <row r="26" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C26" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D26" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="E26" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="23" t="s">
+      <c r="F26" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="G25" s="25" t="s">
+      <c r="G26" s="25" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
     </row>
     <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
@@ -2266,32 +2315,33 @@
     </row>
   </sheetData>
   <autoFilter ref="B4:G4" xr:uid="{6F078BB8-EA6E-4A4D-86BD-D9856AE56810}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:G25">
-      <sortCondition ref="B4:B25"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:G26">
+      <sortCondition ref="B4:B26"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D16" r:id="rId1" xr:uid="{0B6F9ADC-EE7B-CD42-961D-67F77CDF8C1A}"/>
+    <hyperlink ref="D17" r:id="rId1" xr:uid="{0B6F9ADC-EE7B-CD42-961D-67F77CDF8C1A}"/>
     <hyperlink ref="D5" r:id="rId2" xr:uid="{8E5EB032-728D-704B-B5F0-FAC8C55BFE10}"/>
     <hyperlink ref="D7" r:id="rId3" xr:uid="{5221DADD-7AC0-EB4F-A2A7-306F868E3FA1}"/>
     <hyperlink ref="D6" r:id="rId4" xr:uid="{38489070-47F8-F941-A8B1-76D8B375DD92}"/>
-    <hyperlink ref="D12" r:id="rId5" xr:uid="{E65F263A-3188-894D-BA69-E261EE620918}"/>
-    <hyperlink ref="D13" r:id="rId6" xr:uid="{F1544DFD-8672-1C4E-BBD4-3487CA54023F}"/>
-    <hyperlink ref="D14" r:id="rId7" xr:uid="{7A00F97D-130C-5743-A124-269AFEA6396D}"/>
-    <hyperlink ref="D17" r:id="rId8" xr:uid="{85EFFB62-480B-E341-A456-51C6C3B16B94}"/>
-    <hyperlink ref="D18" r:id="rId9" xr:uid="{BEBCF35C-4E7D-3C49-AE74-13F94B34BBC1}"/>
-    <hyperlink ref="D19" r:id="rId10" xr:uid="{C7770802-A95F-8C42-A292-70FA7C3C5319}"/>
-    <hyperlink ref="D22" r:id="rId11" xr:uid="{4415E758-7CEB-874F-AE4A-C6C3ADF74690}"/>
-    <hyperlink ref="D25" r:id="rId12" xr:uid="{53E0A9A6-CA1E-184D-809C-F59EC256D5C5}"/>
+    <hyperlink ref="D13" r:id="rId5" xr:uid="{E65F263A-3188-894D-BA69-E261EE620918}"/>
+    <hyperlink ref="D14" r:id="rId6" xr:uid="{F1544DFD-8672-1C4E-BBD4-3487CA54023F}"/>
+    <hyperlink ref="D15" r:id="rId7" xr:uid="{7A00F97D-130C-5743-A124-269AFEA6396D}"/>
+    <hyperlink ref="D18" r:id="rId8" xr:uid="{85EFFB62-480B-E341-A456-51C6C3B16B94}"/>
+    <hyperlink ref="D19" r:id="rId9" xr:uid="{BEBCF35C-4E7D-3C49-AE74-13F94B34BBC1}"/>
+    <hyperlink ref="D20" r:id="rId10" xr:uid="{C7770802-A95F-8C42-A292-70FA7C3C5319}"/>
+    <hyperlink ref="D23" r:id="rId11" xr:uid="{4415E758-7CEB-874F-AE4A-C6C3ADF74690}"/>
+    <hyperlink ref="D26" r:id="rId12" xr:uid="{53E0A9A6-CA1E-184D-809C-F59EC256D5C5}"/>
     <hyperlink ref="D8" r:id="rId13" xr:uid="{FCF5A9D5-945D-8445-A61E-5BCEB328BDE4}"/>
-    <hyperlink ref="D24" r:id="rId14" xr:uid="{34CF9B78-6FF2-834C-8BF0-B88C37A72689}"/>
-    <hyperlink ref="D21" r:id="rId15" xr:uid="{9498ACDE-D79A-794C-B5F1-41EA1C52D72C}"/>
-    <hyperlink ref="D20" r:id="rId16" xr:uid="{02600190-F3FB-FA45-9502-0B47CDBA9722}"/>
+    <hyperlink ref="D25" r:id="rId14" xr:uid="{34CF9B78-6FF2-834C-8BF0-B88C37A72689}"/>
+    <hyperlink ref="D22" r:id="rId15" xr:uid="{9498ACDE-D79A-794C-B5F1-41EA1C52D72C}"/>
+    <hyperlink ref="D21" r:id="rId16" xr:uid="{02600190-F3FB-FA45-9502-0B47CDBA9722}"/>
+    <hyperlink ref="D10" r:id="rId17" xr:uid="{3D67F25E-459B-844A-8CA3-8A32D89D111C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId17"/>
-  <drawing r:id="rId18"/>
-  <legacyDrawing r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId18"/>
+  <drawing r:id="rId19"/>
+  <legacyDrawing r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -2299,8 +2349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2366,103 +2416,103 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="10" t="str">
         <f>IF('01 - COTS List'!B10="","","|**"&amp;'01 - COTS List'!B10&amp;"**|"&amp;'01 - COTS List'!C10&amp;"|"&amp;'01 - COTS List'!D10&amp;"|"&amp;'01 - COTS List'!E10&amp;"|"&amp;'01 - COTS List'!F10&amp;"|")</f>
-        <v>|**express**|4.*.*|https://www.npmjs.com/package/express|MIT|Express.js, or simply Express, is a web application framework for Node.js, released as free and open-source software under the MIT License.|</v>
+        <v>|**dotenv**|6.*.*|https://www.npmjs.com/package/dotenv|BSD-2-Clause|Dotenv is a zero-dependency module that loads environment variables from a .env file into process.env|</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="10" t="str">
         <f>IF('01 - COTS List'!B11="","","|**"&amp;'01 - COTS List'!B11&amp;"**|"&amp;'01 - COTS List'!C11&amp;"|"&amp;'01 - COTS List'!D11&amp;"|"&amp;'01 - COTS List'!E11&amp;"|"&amp;'01 - COTS List'!F11&amp;"|")</f>
-        <v>|**helmet**|3.*.*|https://www.npmjs.com/package/helmet|MIT|Helmet helps you secure your Express apps by setting various HTTP headers.|</v>
+        <v>|**express**|4.*.*|https://www.npmjs.com/package/express|MIT|Express.js, or simply Express, is a web application framework for Node.js, released as free and open-source software under the MIT License.|</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="str">
         <f>IF('01 - COTS List'!B12="","","|**"&amp;'01 - COTS List'!B12&amp;"**|"&amp;'01 - COTS List'!C12&amp;"|"&amp;'01 - COTS List'!D12&amp;"|"&amp;'01 - COTS List'!E12&amp;"|"&amp;'01 - COTS List'!F12&amp;"|")</f>
-        <v>|**jwt-decode**|2.*.*|https://www.npmjs.com/package/jwt-decode|MIT|jwt-decode is a small browser library that helps decoding JWTs token which are Base64Url encoded.|</v>
+        <v>|**helmet**|3.*.*|https://www.npmjs.com/package/helmet|MIT|Helmet helps you secure your Express apps by setting various HTTP headers.|</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" s="10" t="str">
         <f>IF('01 - COTS List'!B13="","","|**"&amp;'01 - COTS List'!B13&amp;"**|"&amp;'01 - COTS List'!C13&amp;"|"&amp;'01 - COTS List'!D13&amp;"|"&amp;'01 - COTS List'!E13&amp;"|"&amp;'01 - COTS List'!F13&amp;"|")</f>
-        <v>|**lodash**|4.*.*|https://www.npmjs.com/package/lodash|MIT|The Lodash library exported as Node.js modules.|</v>
+        <v>|**jwt-decode**|2.*.*|https://www.npmjs.com/package/jwt-decode|MIT|jwt-decode is a small browser library that helps decoding JWTs token which are Base64Url encoded.|</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="str">
         <f>IF('01 - COTS List'!B14="","","|**"&amp;'01 - COTS List'!B14&amp;"**|"&amp;'01 - COTS List'!C14&amp;"|"&amp;'01 - COTS List'!D14&amp;"|"&amp;'01 - COTS List'!E14&amp;"|"&amp;'01 - COTS List'!F14&amp;"|")</f>
-        <v>|**log4js**|3.*.*|https://www.npmjs.com/package/log4js|MIT|This is a conversion of the log4js framework to work with node|</v>
+        <v>|**lodash**|4.*.*|https://www.npmjs.com/package/lodash|MIT|The Lodash library exported as Node.js modules.|</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="str">
         <f>IF('01 - COTS List'!B15="","","|**"&amp;'01 - COTS List'!B15&amp;"**|"&amp;'01 - COTS List'!C15&amp;"|"&amp;'01 - COTS List'!D15&amp;"|"&amp;'01 - COTS List'!E15&amp;"|"&amp;'01 - COTS List'!F15&amp;"|")</f>
-        <v>|**mime**|2.*.*|https://www.npmjs.com/package/mime|MIT|A comprehensive, compact MIME type module.|</v>
+        <v>|**log4js**|3.*.*|https://www.npmjs.com/package/log4js|MIT|This is a conversion of the log4js framework to work with node|</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="str">
         <f>IF('01 - COTS List'!B16="","","|**"&amp;'01 - COTS List'!B16&amp;"**|"&amp;'01 - COTS List'!C16&amp;"|"&amp;'01 - COTS List'!D16&amp;"|"&amp;'01 - COTS List'!E16&amp;"|"&amp;'01 - COTS List'!F16&amp;"|")</f>
-        <v>|**Node**|10.*.*|https://nodejs.org/en/|MIT|Node.js is a JavaScript runtime built on Chrome's V8 JavaScript engine.|</v>
+        <v>|**mime**|2.*.*|https://www.npmjs.com/package/mime|MIT|A comprehensive, compact MIME type module.|</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="str">
         <f>IF('01 - COTS List'!B17="","","|**"&amp;'01 - COTS List'!B17&amp;"**|"&amp;'01 - COTS List'!C17&amp;"|"&amp;'01 - COTS List'!D17&amp;"|"&amp;'01 - COTS List'!E17&amp;"|"&amp;'01 - COTS List'!F17&amp;"|")</f>
-        <v>|**passport**|0.*.*|https://www.npmjs.com/package/passport|MIT|Passport's sole purpose is to authenticate requests, which it does through an extensible set of plugins known as strategies.|</v>
+        <v>|**Node**|10.*.*|https://nodejs.org/en/|MIT|Node.js is a JavaScript runtime built on Chrome's V8 JavaScript engine.|</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="str">
         <f>IF('01 - COTS List'!B18="","","|**"&amp;'01 - COTS List'!B18&amp;"**|"&amp;'01 - COTS List'!C18&amp;"|"&amp;'01 - COTS List'!D18&amp;"|"&amp;'01 - COTS List'!E18&amp;"|"&amp;'01 - COTS List'!F18&amp;"|")</f>
-        <v>|**passport-jwt**|4.*.*|https://www.npmjs.com/package/passport-jwt|MIT|A Passport strategy for authenticating with a JSON Web Token.|</v>
+        <v>|**passport**|0.*.*|https://www.npmjs.com/package/passport|MIT|Passport's sole purpose is to authenticate requests, which it does through an extensible set of plugins known as strategies.|</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="str">
         <f>IF('01 - COTS List'!B19="","","|**"&amp;'01 - COTS List'!B19&amp;"**|"&amp;'01 - COTS List'!C19&amp;"|"&amp;'01 - COTS List'!D19&amp;"|"&amp;'01 - COTS List'!E19&amp;"|"&amp;'01 - COTS List'!F19&amp;"|")</f>
-        <v>|**pg**|7.*.*|https://www.npmjs.com/package/pg|MIT|Non-blocking PostgreSQL client for Node.js. Pure JavaScript and optional native libpq bindings.|</v>
+        <v>|**passport-jwt**|4.*.*|https://www.npmjs.com/package/passport-jwt|MIT|A Passport strategy for authenticating with a JSON Web Token.|</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="str">
         <f>IF('01 - COTS List'!B20="","","|**"&amp;'01 - COTS List'!B20&amp;"**|"&amp;'01 - COTS List'!C20&amp;"|"&amp;'01 - COTS List'!D20&amp;"|"&amp;'01 - COTS List'!E20&amp;"|"&amp;'01 - COTS List'!F20&amp;"|")</f>
-        <v>|**PostGIS**|2.*.*|https://postgis.net/|GPLv2|PostGIS is a spatial database extender for PostgreSQL object-relational database. It adds support for geographic objects allowing location queries to be run in SQL.|</v>
+        <v>|**pg**|7.*.*|https://www.npmjs.com/package/pg|MIT|Non-blocking PostgreSQL client for Node.js. Pure JavaScript and optional native libpq bindings.|</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="str">
         <f>IF('01 - COTS List'!B21="","","|**"&amp;'01 - COTS List'!B21&amp;"**|"&amp;'01 - COTS List'!C21&amp;"|"&amp;'01 - COTS List'!D21&amp;"|"&amp;'01 - COTS List'!E21&amp;"|"&amp;'01 - COTS List'!F21&amp;"|")</f>
-        <v>|**PostgreSQL**|9.*|https://www.postgresql.org/|PostgreSQL License|PostgreSQL, is an object-relational database management system (ORDBMS) with an emphasis on extensibility and standards compliance|</v>
+        <v>|**PostGIS**|2.*.*|https://postgis.net/|GPLv2|PostGIS is a spatial database extender for PostgreSQL object-relational database. It adds support for geographic objects allowing location queries to be run in SQL.|</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="10" t="str">
         <f>IF('01 - COTS List'!B22="","","|**"&amp;'01 - COTS List'!B22&amp;"**|"&amp;'01 - COTS List'!C22&amp;"|"&amp;'01 - COTS List'!D22&amp;"|"&amp;'01 - COTS List'!E22&amp;"|"&amp;'01 - COTS List'!F22&amp;"|")</f>
-        <v>|**sequelize**|4.*.*|https://www.npmjs.com/package/sequelize|MIT|Sequelize is a promise-based Node.js ORM for Postgres, MySQL, SQLite and Microsoft SQL Server. It features solid transaction support, relations, read replication and more.|</v>
+        <v>|**PostgreSQL**|9.*|https://www.postgresql.org/|PostgreSQL License|PostgreSQL, is an object-relational database management system (ORDBMS) with an emphasis on extensibility and standards compliance|</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" s="10" t="str">
         <f>IF('01 - COTS List'!B23="","","|**"&amp;'01 - COTS List'!B23&amp;"**|"&amp;'01 - COTS List'!C23&amp;"|"&amp;'01 - COTS List'!D23&amp;"|"&amp;'01 - COTS List'!E23&amp;"|"&amp;'01 - COTS List'!F23&amp;"|")</f>
-        <v>|**swagger-ui-express**|3.*.*|https://www.npmjs.com/package/swagger-ui-express|MIT|API documentation generator|</v>
+        <v>|**sequelize**|4.*.*|https://www.npmjs.com/package/sequelize|MIT|Sequelize is a promise-based Node.js ORM for Postgres, MySQL, SQLite and Microsoft SQL Server. It features solid transaction support, relations, read replication and more.|</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" s="10" t="str">
         <f>IF('01 - COTS List'!B24="","","|**"&amp;'01 - COTS List'!B24&amp;"**|"&amp;'01 - COTS List'!C24&amp;"|"&amp;'01 - COTS List'!D24&amp;"|"&amp;'01 - COTS List'!E24&amp;"|"&amp;'01 - COTS List'!F24&amp;"|")</f>
-        <v>|**useragent**|2.*.*|https://www.npmjs.com/package/useragent|MIT|Useragent originated as port of browserscope.org's user agent parser project also known as ua-parser.|</v>
+        <v>|**swagger-ui-express**|3.*.*|https://www.npmjs.com/package/swagger-ui-express|MIT|API documentation generator|</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" s="10" t="str">
         <f>IF('01 - COTS List'!B25="","","|**"&amp;'01 - COTS List'!B25&amp;"**|"&amp;'01 - COTS List'!C25&amp;"|"&amp;'01 - COTS List'!D25&amp;"|"&amp;'01 - COTS List'!E25&amp;"|"&amp;'01 - COTS List'!F25&amp;"|")</f>
-        <v>|**yamljs**|0.*.*|https://www.npmjs.com/package/yamljs|MIT|Standalone JavaScript YAML 1.2 Parser &amp; Encoder. Works under node.js and all major browsers. Also brings command line YAML/JSON conversion tools.|</v>
+        <v>|**useragent**|2.*.*|https://www.npmjs.com/package/useragent|MIT|Useragent originated as port of browserscope.org's user agent parser project also known as ua-parser.|</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" s="10" t="str">
         <f>IF('01 - COTS List'!B26="","","|**"&amp;'01 - COTS List'!B26&amp;"**|"&amp;'01 - COTS List'!C26&amp;"|"&amp;'01 - COTS List'!D26&amp;"|"&amp;'01 - COTS List'!E26&amp;"|"&amp;'01 - COTS List'!F26&amp;"|")</f>
-        <v/>
+        <v>|**yamljs**|0.*.*|https://www.npmjs.com/package/yamljs|MIT|Standalone JavaScript YAML 1.2 Parser &amp; Encoder. Works under node.js and all major browsers. Also brings command line YAML/JSON conversion tools.|</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>